<commit_message>
caso 4 restriccion comentada x2
</commit_message>
<xml_diff>
--- a/caso 4/caso4_excel.xlsx
+++ b/caso 4/caso4_excel.xlsx
@@ -1199,13 +1199,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1213,7 +1213,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>125485.7142857143</v>
+        <v>126600</v>
       </c>
     </row>
     <row r="5">
@@ -1223,13 +1223,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1247,13 +1247,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>236914.2857142857</v>
+        <v>237600</v>
       </c>
     </row>
     <row r="7">
@@ -1271,13 +1271,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1295,13 +1295,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1309,7 +1309,7 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>259200</v>
+        <v>260100</v>
       </c>
       <c r="J8" s="20" t="n"/>
     </row>
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>8.365714285714287</v>
+        <v>8.44</v>
       </c>
     </row>
     <row r="12">
@@ -1386,7 +1386,7 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>9.476571428571429</v>
+        <v>9.504</v>
       </c>
     </row>
     <row r="14">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>9.6</v>
+        <v>9.633333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
caso 4 restriccion FINAL
</commit_message>
<xml_diff>
--- a/caso 4/caso4_excel.xlsx
+++ b/caso 4/caso4_excel.xlsx
@@ -1213,7 +1213,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>126600</v>
+        <v>152600</v>
       </c>
     </row>
     <row r="5">
@@ -1226,7 +1226,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>147300</v>
+        <v>154800</v>
       </c>
     </row>
     <row r="6">
@@ -1274,7 +1274,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>207300</v>
+        <v>210050</v>
       </c>
     </row>
     <row r="8">
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>8.44</v>
+        <v>10.17333333333333</v>
       </c>
     </row>
     <row r="12">
@@ -1368,7 +1368,7 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>4.91</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="13">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>5.1825</v>
+        <v>5.25125</v>
       </c>
     </row>
     <row r="15">

</xml_diff>